<commit_message>
First working draft - Not nicely formatted
</commit_message>
<xml_diff>
--- a/images/CRS-30201-50150-ST-HB-DOD-30201-50150-LT-HE-GG-001-00-00-019 (1).xlsx
+++ b/images/CRS-30201-50150-ST-HB-DOD-30201-50150-LT-HE-GG-001-00-00-019 (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\5.0 Project Management\5.09 Project Deliverables\5.9.1 Project Plan &amp; Engineering Execution Plan\Rev B\03. Native File\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aamir406/Documents/AVENIR/crs-ai/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878AAB8A-893F-49E2-98DD-11CC940A57DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E0C93D-2654-7441-8186-23027303B8C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{A58DD4C1-53AF-419B-A997-6826F3633C93}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" xr2:uid="{A58DD4C1-53AF-419B-A997-6826F3633C93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$88</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$11:$11</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Received Date:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPANY Comment </t>
   </si>
   <si>
     <t>ENGINEERING CONTRACTOR Response</t>
@@ -628,6 +625,9 @@
   </si>
   <si>
     <t>REVISION A (ADNOCGP-WTRAN-002723)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -700,13 +700,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -957,14 +957,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -992,7 +986,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1001,13 +995,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1016,28 +1023,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1049,7 +1062,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1061,32 +1077,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1160,7 +1170,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="18360262" y="169129"/>
+          <a:off x="20885660" y="169129"/>
           <a:ext cx="784215" cy="870356"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="5513705" cy="8628380"/>
@@ -4194,9 +4204,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>752475</xdr:colOff>
+          <xdr:colOff>749300</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
@@ -4234,14 +4244,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -4261,9 +4271,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1016000</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>241300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -4301,14 +4311,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -4328,7 +4338,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>1009650</xdr:colOff>
+          <xdr:colOff>1016000</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -4336,7 +4346,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4368,14 +4378,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -4395,15 +4405,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>733425</xdr:colOff>
+          <xdr:colOff>736600</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>962025</xdr:colOff>
+          <xdr:colOff>965200</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4435,14 +4445,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -4564,7 +4574,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>1009650</xdr:colOff>
+          <xdr:colOff>1016000</xdr:colOff>
           <xdr:row>86</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -4572,7 +4582,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>86</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:rowOff>254000</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4604,14 +4614,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -4931,2229 +4941,2231 @@
   </sheetPr>
   <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="88" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="8" width="45.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="8" width="45.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="90.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="31" t="s">
+    <row r="1" spans="1:11" ht="91" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="44"/>
+    </row>
+    <row r="3" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="38"/>
-    </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="22"/>
+      <c r="K3" s="5">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="30" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="7">
-        <v>45772</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="22"/>
+      <c r="K4" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="22"/>
+      <c r="K5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="32" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="40"/>
+      <c r="K6" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="40"/>
+      <c r="K7" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="C8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
+    </row>
+    <row r="9" spans="1:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="46"/>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
         <v>1</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="8" t="s">
+      <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="34"/>
-      <c r="K6" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="34"/>
-      <c r="K7" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
-    </row>
-    <row r="9" spans="1:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="23"/>
-    </row>
-    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
-    </row>
-    <row r="11" spans="1:11" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11" s="42"/>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
         <f>A12+1</f>
         <v>2</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="F13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="E13" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+    </row>
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
         <f t="shared" ref="A14:A17" si="0">A13+1</f>
         <v>3</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-    </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="C14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+    </row>
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-    </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="D15" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+    </row>
+    <row r="16" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-    </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="D16" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+    </row>
+    <row r="17" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-    </row>
-    <row r="18" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+    </row>
+    <row r="18" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
         <f>A17+1</f>
         <v>7</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-    </row>
-    <row r="19" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="D18" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+    </row>
+    <row r="19" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
         <f>A18+1</f>
         <v>8</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="14" t="s">
+      <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+    </row>
+    <row r="20" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>9</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E19" s="14" t="s">
+      <c r="C20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-    </row>
-    <row r="20" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>9</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="14" t="s">
+      <c r="E20" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-    </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+    </row>
+    <row r="21" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
         <f>A20+1</f>
         <v>10</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="F21" s="14" t="s">
+      <c r="D21" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
-    </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="E21" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+    </row>
+    <row r="22" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
         <f t="shared" ref="A22" si="1">A21+1</f>
         <v>11</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
-    </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+    </row>
+    <row r="23" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
         <f>A22+1</f>
         <v>12</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F23" s="14" t="s">
+      <c r="B23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-    </row>
-    <row r="24" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="E23" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+    </row>
+    <row r="24" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
         <f>A23+1</f>
         <v>13</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F24" s="14" t="s">
+      <c r="B24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-    </row>
-    <row r="25" spans="1:11" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="E24" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+    </row>
+    <row r="25" spans="1:11" s="2" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
         <f t="shared" ref="A25:A87" si="2">A24+1</f>
         <v>14</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-    </row>
-    <row r="26" spans="1:11" s="4" customFormat="1" ht="255" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="B25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+    </row>
+    <row r="26" spans="1:11" s="2" customFormat="1" ht="256" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
         <f>A25+1</f>
         <v>15</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-    </row>
-    <row r="27" spans="1:11" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="D26" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+    </row>
+    <row r="27" spans="1:11" s="2" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F27" s="14" t="s">
+      <c r="B27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-    </row>
-    <row r="28" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="E27" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+    </row>
+    <row r="28" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
         <f>A27+1</f>
         <v>17</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="F28" s="14" t="s">
+      <c r="D28" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
-    </row>
-    <row r="29" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="E28" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+    </row>
+    <row r="29" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-    </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="B29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+    </row>
+    <row r="30" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-    </row>
-    <row r="31" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="B30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+    </row>
+    <row r="31" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-    </row>
-    <row r="32" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+      <c r="B31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+    </row>
+    <row r="32" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-    </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="B32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+    </row>
+    <row r="33" spans="1:11" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-    </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
+      <c r="D33" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+    </row>
+    <row r="34" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-    </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="B34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+    </row>
+    <row r="35" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-    </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+      <c r="B35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+    </row>
+    <row r="36" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-    </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+      <c r="B36" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
+    </row>
+    <row r="37" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-    </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+      <c r="B37" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+    </row>
+    <row r="38" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="43"/>
-    </row>
-    <row r="39" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="B38" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+    </row>
+    <row r="39" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="43"/>
-    </row>
-    <row r="40" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+      <c r="B39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="45"/>
+    </row>
+    <row r="40" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A40" s="7">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="43"/>
-    </row>
-    <row r="41" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+      <c r="B40" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="45"/>
+    </row>
+    <row r="41" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A41" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="43"/>
-    </row>
-    <row r="42" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+      <c r="B41" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="45"/>
+      <c r="K41" s="45"/>
+    </row>
+    <row r="42" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A42" s="7">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="43"/>
-      <c r="K42" s="43"/>
-    </row>
-    <row r="43" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+      <c r="D42" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="45"/>
+    </row>
+    <row r="43" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="7">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-    </row>
-    <row r="44" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
+      <c r="B43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="45"/>
+    </row>
+    <row r="44" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="43"/>
-    </row>
-    <row r="45" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+      <c r="B44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="45"/>
+    </row>
+    <row r="45" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A45" s="7">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-    </row>
-    <row r="46" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
+      <c r="B45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="45"/>
+    </row>
+    <row r="46" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="43"/>
-      <c r="K46" s="43"/>
-    </row>
-    <row r="47" spans="1:11" s="4" customFormat="1" ht="195" x14ac:dyDescent="0.25">
-      <c r="A47" s="9">
+      <c r="B46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="45"/>
+    </row>
+    <row r="47" spans="1:11" s="2" customFormat="1" ht="160" x14ac:dyDescent="0.2">
+      <c r="A47" s="7">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F47" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="43"/>
-    </row>
-    <row r="48" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9">
+      <c r="B47" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="45"/>
+      <c r="K47" s="45"/>
+    </row>
+    <row r="48" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="7">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="43"/>
-    </row>
-    <row r="49" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
+      <c r="D48" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="45"/>
+    </row>
+    <row r="49" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A49" s="7">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="F49" s="14" t="s">
+      <c r="B49" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-    </row>
-    <row r="50" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+      <c r="E49" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="45"/>
+    </row>
+    <row r="50" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A50" s="7">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="F50" s="14" t="s">
+      <c r="B50" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-    </row>
-    <row r="51" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="9">
+      <c r="E50" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="45"/>
+    </row>
+    <row r="51" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A51" s="7">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C51" s="14" t="s">
+      <c r="B51" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D51" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="E51" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="43"/>
-    </row>
-    <row r="52" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
+      <c r="C51" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="45"/>
+    </row>
+    <row r="52" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="7">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C52" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="43"/>
-      <c r="K52" s="43"/>
-    </row>
-    <row r="53" spans="1:11" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A53" s="9">
+      <c r="D52" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="45"/>
+    </row>
+    <row r="53" spans="1:11" s="2" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A53" s="7">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C53" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D53" s="14" t="s">
+      <c r="B53" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F53" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E53" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="43"/>
-      <c r="K53" s="43"/>
-    </row>
-    <row r="54" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="45"/>
+      <c r="K53" s="45"/>
+    </row>
+    <row r="54" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A54" s="7">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C54" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C54" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="43"/>
-      <c r="K54" s="43"/>
-    </row>
-    <row r="55" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
+      <c r="D54" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="45"/>
+    </row>
+    <row r="55" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="7">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C55" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F55" s="14" t="s">
+      <c r="D55" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="43"/>
-      <c r="K55" s="43"/>
-    </row>
-    <row r="56" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
+      <c r="E55" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="45"/>
+      <c r="K55" s="45"/>
+    </row>
+    <row r="56" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="7">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="43"/>
-      <c r="K56" s="43"/>
-    </row>
-    <row r="57" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="9">
+      <c r="B56" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="45"/>
+    </row>
+    <row r="57" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="7">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F57" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="43"/>
-      <c r="K57" s="43"/>
-    </row>
-    <row r="58" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
+      <c r="B57" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="45"/>
+      <c r="K57" s="45"/>
+    </row>
+    <row r="58" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="7">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D58" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F58" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="43"/>
-      <c r="K58" s="43"/>
-    </row>
-    <row r="59" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="9">
+      <c r="B58" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="45"/>
+    </row>
+    <row r="59" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A59" s="7">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C59" s="14" t="s">
+      <c r="B59" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D59" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="43"/>
-      <c r="K59" s="43"/>
-    </row>
-    <row r="60" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="9">
+      <c r="C59" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="45"/>
+      <c r="K59" s="45"/>
+    </row>
+    <row r="60" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A60" s="7">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D60" s="14" t="s">
+      <c r="D60" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="F60" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E60" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="43"/>
-      <c r="K60" s="43"/>
-    </row>
-    <row r="61" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A61" s="9">
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="45"/>
+      <c r="K60" s="45"/>
+    </row>
+    <row r="61" spans="1:11" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A61" s="7">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C61" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F61" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="43"/>
-      <c r="K61" s="43"/>
-    </row>
-    <row r="62" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="9">
+      <c r="D61" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="45"/>
+      <c r="K61" s="45"/>
+    </row>
+    <row r="62" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A62" s="7">
         <f t="shared" si="2"/>
         <v>51</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C62" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F62" s="14" t="s">
+      <c r="D62" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="43"/>
-      <c r="K62" s="43"/>
-    </row>
-    <row r="63" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="9">
+      <c r="E62" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="45"/>
+      <c r="K62" s="45"/>
+    </row>
+    <row r="63" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A63" s="7">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D63" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F63" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="43"/>
-      <c r="K63" s="43"/>
-    </row>
-    <row r="64" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="9">
+      <c r="B63" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="45"/>
+      <c r="K63" s="45"/>
+    </row>
+    <row r="64" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A64" s="7">
         <f t="shared" si="2"/>
         <v>53</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="E64" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F64" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="43"/>
-      <c r="K64" s="43"/>
-    </row>
-    <row r="65" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="9">
+      <c r="B64" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="45"/>
+      <c r="K64" s="45"/>
+    </row>
+    <row r="65" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A65" s="7">
         <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C65" s="14" t="s">
+      <c r="B65" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D65" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="43"/>
-      <c r="K65" s="43"/>
-    </row>
-    <row r="66" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="9">
+      <c r="C65" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="45"/>
+      <c r="K65" s="45"/>
+    </row>
+    <row r="66" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="7">
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C66" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D66" s="14" t="s">
+      <c r="D66" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F66" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E66" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F66" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="43"/>
-      <c r="K66" s="43"/>
-    </row>
-    <row r="67" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="9">
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="45"/>
+      <c r="K66" s="45"/>
+    </row>
+    <row r="67" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A67" s="7">
         <f t="shared" si="2"/>
         <v>56</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D67" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E67" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F67" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="43"/>
-      <c r="K67" s="43"/>
-    </row>
-    <row r="68" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="9">
+      <c r="B67" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="45"/>
+      <c r="K67" s="45"/>
+    </row>
+    <row r="68" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A68" s="7">
         <f t="shared" si="2"/>
         <v>57</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C68" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D68" s="14" t="s">
+      <c r="B68" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F68" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E68" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F68" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="43"/>
-      <c r="K68" s="43"/>
-    </row>
-    <row r="69" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="9">
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="45"/>
+      <c r="K68" s="45"/>
+    </row>
+    <row r="69" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A69" s="7">
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E69" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F69" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="43"/>
-      <c r="K69" s="43"/>
-    </row>
-    <row r="70" spans="1:11" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="9">
+      <c r="B69" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="45"/>
+      <c r="K69" s="45"/>
+    </row>
+    <row r="70" spans="1:11" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="7">
         <f t="shared" si="2"/>
         <v>59</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C70" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C70" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D70" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="E70" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F70" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="43"/>
-      <c r="K70" s="43"/>
-    </row>
-    <row r="71" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A71" s="9">
+      <c r="D70" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="45"/>
+      <c r="K70" s="45"/>
+    </row>
+    <row r="71" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A71" s="7">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C71" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D71" s="14" t="s">
+      <c r="B71" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F71" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E71" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F71" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="43"/>
-      <c r="K71" s="43"/>
-    </row>
-    <row r="72" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="9">
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="45"/>
+      <c r="K71" s="45"/>
+    </row>
+    <row r="72" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A72" s="7">
         <f t="shared" si="2"/>
         <v>61</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C72" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C72" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="D72" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E72" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F72" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="43"/>
-      <c r="K72" s="43"/>
-    </row>
-    <row r="73" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A73" s="9">
+      <c r="D72" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="45"/>
+      <c r="K72" s="45"/>
+    </row>
+    <row r="73" spans="1:11" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A73" s="7">
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C73" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C73" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D73" s="14" t="s">
+      <c r="D73" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F73" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E73" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F73" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="43"/>
-      <c r="K73" s="43"/>
-    </row>
-    <row r="74" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="9">
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
+      <c r="J73" s="45"/>
+      <c r="K73" s="45"/>
+    </row>
+    <row r="74" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A74" s="7">
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C74" s="14" t="s">
+      <c r="B74" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D74" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="E74" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F74" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="43"/>
-      <c r="K74" s="43"/>
-    </row>
-    <row r="75" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A75" s="9">
+      <c r="C74" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F74" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
+      <c r="J74" s="45"/>
+      <c r="K74" s="45"/>
+    </row>
+    <row r="75" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A75" s="7">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C75" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C75" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D75" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E75" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F75" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G75" s="14"/>
-      <c r="H75" s="14"/>
-      <c r="I75" s="14"/>
-      <c r="J75" s="43"/>
-      <c r="K75" s="43"/>
-    </row>
-    <row r="76" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A76" s="9">
+      <c r="D75" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F75" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="12"/>
+      <c r="J75" s="45"/>
+      <c r="K75" s="45"/>
+    </row>
+    <row r="76" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A76" s="7">
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C76" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C76" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D76" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E76" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F76" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
-      <c r="I76" s="14"/>
-      <c r="J76" s="43"/>
-      <c r="K76" s="43"/>
-    </row>
-    <row r="77" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="9">
+      <c r="D76" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F76" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="45"/>
+      <c r="K76" s="45"/>
+    </row>
+    <row r="77" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A77" s="7">
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C77" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="D77" s="14" t="s">
+      <c r="B77" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E77" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F77" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E77" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F77" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
-      <c r="I77" s="14"/>
-      <c r="J77" s="43"/>
-      <c r="K77" s="43"/>
-    </row>
-    <row r="78" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="9">
+      <c r="G77" s="12"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="12"/>
+      <c r="J77" s="45"/>
+      <c r="K77" s="45"/>
+    </row>
+    <row r="78" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" s="7">
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
-      <c r="B78" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C78" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="D78" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E78" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F78" s="14" t="s">
+      <c r="B78" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D78" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
-      <c r="I78" s="14"/>
-      <c r="J78" s="43"/>
-      <c r="K78" s="43"/>
-    </row>
-    <row r="79" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="9">
+      <c r="E78" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F78" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="45"/>
+      <c r="K78" s="45"/>
+    </row>
+    <row r="79" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A79" s="7">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C79" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D79" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E79" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F79" s="14" t="s">
+      <c r="B79" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D79" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="14"/>
-      <c r="J79" s="43"/>
-      <c r="K79" s="43"/>
-    </row>
-    <row r="80" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="9">
+      <c r="E79" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F79" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="45"/>
+      <c r="K79" s="45"/>
+    </row>
+    <row r="80" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="7">
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C80" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D80" s="14" t="s">
+      <c r="B80" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E80" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F80" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E80" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F80" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="14"/>
-      <c r="J80" s="43"/>
-      <c r="K80" s="43"/>
-    </row>
-    <row r="81" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A81" s="9">
+      <c r="G80" s="12"/>
+      <c r="H80" s="12"/>
+      <c r="I80" s="12"/>
+      <c r="J80" s="45"/>
+      <c r="K80" s="45"/>
+    </row>
+    <row r="81" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A81" s="7">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="B81" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C81" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D81" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="E81" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F81" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="14"/>
-      <c r="J81" s="43"/>
-      <c r="K81" s="43"/>
-    </row>
-    <row r="82" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A82" s="9">
+      <c r="B81" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E81" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F81" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="12"/>
+      <c r="J81" s="45"/>
+      <c r="K81" s="45"/>
+    </row>
+    <row r="82" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A82" s="7">
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C82" s="14" t="s">
+      <c r="B82" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D82" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E82" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F82" s="14" t="s">
+      <c r="C82" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D82" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G82" s="14"/>
-      <c r="H82" s="14"/>
-      <c r="I82" s="14"/>
-      <c r="J82" s="43"/>
-      <c r="K82" s="43"/>
-    </row>
-    <row r="83" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A83" s="9">
+      <c r="E82" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F82" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="45"/>
+      <c r="K82" s="45"/>
+    </row>
+    <row r="83" spans="1:11" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A83" s="7">
         <f t="shared" si="2"/>
         <v>72</v>
       </c>
-      <c r="B83" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C83" s="14" t="s">
+      <c r="B83" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D83" s="14" t="s">
+      <c r="C83" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E83" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F83" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E83" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F83" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G83" s="14"/>
-      <c r="H83" s="14"/>
-      <c r="I83" s="14"/>
-      <c r="J83" s="43"/>
-      <c r="K83" s="43"/>
-    </row>
-    <row r="84" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="9">
+      <c r="G83" s="12"/>
+      <c r="H83" s="12"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="45"/>
+      <c r="K83" s="45"/>
+    </row>
+    <row r="84" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A84" s="7">
         <f t="shared" si="2"/>
         <v>73</v>
       </c>
-      <c r="B84" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C84" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="D84" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E84" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F84" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="14"/>
-      <c r="J84" s="43"/>
-      <c r="K84" s="43"/>
-    </row>
-    <row r="85" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="9">
+      <c r="B84" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E84" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F84" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="45"/>
+      <c r="K84" s="45"/>
+    </row>
+    <row r="85" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="7">
         <f t="shared" si="2"/>
         <v>74</v>
       </c>
-      <c r="B85" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D85" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E85" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F85" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="14"/>
-      <c r="J85" s="43"/>
-      <c r="K85" s="43"/>
-    </row>
-    <row r="86" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="9">
+      <c r="B85" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E85" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F85" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="45"/>
+      <c r="K85" s="45"/>
+    </row>
+    <row r="86" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A86" s="7">
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="B86" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C86" s="14" t="s">
+      <c r="B86" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D86" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="E86" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F86" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="14"/>
-      <c r="J86" s="43"/>
-      <c r="K86" s="43"/>
-    </row>
-    <row r="87" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="9">
+      <c r="C86" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E86" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F86" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G86" s="12"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="12"/>
+      <c r="J86" s="45"/>
+      <c r="K86" s="45"/>
+    </row>
+    <row r="87" spans="1:11" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A87" s="7">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C87" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C87" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D87" s="14" t="s">
+      <c r="D87" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E87" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F87" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E87" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F87" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="14"/>
-      <c r="J87" s="43"/>
-      <c r="K87" s="43"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="44" t="s">
-        <v>166</v>
-      </c>
-      <c r="B88" s="44"/>
-      <c r="C88" s="44"/>
-      <c r="D88" s="44"/>
-      <c r="E88" s="44"/>
-      <c r="F88" s="44"/>
-      <c r="G88" s="44"/>
-      <c r="H88" s="44"/>
-      <c r="I88" s="44"/>
-      <c r="J88" s="44"/>
-      <c r="K88" s="44"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="12"/>
+      <c r="I87" s="12"/>
+      <c r="J87" s="45"/>
+      <c r="K87" s="45"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="B88" s="48"/>
+      <c r="C88" s="48"/>
+      <c r="D88" s="48"/>
+      <c r="E88" s="48"/>
+      <c r="F88" s="48"/>
+      <c r="G88" s="48"/>
+      <c r="H88" s="48"/>
+      <c r="I88" s="48"/>
+      <c r="J88" s="48"/>
+      <c r="K88" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="101">
@@ -7266,7 +7278,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.31496062992125984" bottom="0.31496062992125984" header="0.51181102362204722" footer="0.19685039370078741"/>
-  <pageSetup paperSize="8" scale="69" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="65" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;L&amp;"arial,Regular"&amp;1&amp;K737373
 </oddHeader>
@@ -7289,9 +7301,9 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>752475</xdr:colOff>
+                    <xdr:colOff>749300</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
@@ -7311,9 +7323,9 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1016000</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>241300</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
@@ -7333,7 +7345,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>1009650</xdr:colOff>
+                    <xdr:colOff>1016000</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -7341,7 +7353,7 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7355,15 +7367,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>733425</xdr:colOff>
+                    <xdr:colOff>736600</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>962025</xdr:colOff>
+                    <xdr:colOff>965200</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7377,7 +7389,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>1009650</xdr:colOff>
+                    <xdr:colOff>1016000</xdr:colOff>
                     <xdr:row>86</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -7385,7 +7397,7 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>86</xdr:row>
-                    <xdr:rowOff>257175</xdr:rowOff>
+                    <xdr:rowOff>254000</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>